<commit_message>
working project that I want
</commit_message>
<xml_diff>
--- a/data_test_input/test_book.xlsx
+++ b/data_test_input/test_book.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,26 +541,38 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v/>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="n">
-        <v/>
-      </c>
-      <c r="E1" t="n">
-        <v/>
-      </c>
-      <c r="F1" t="n">
-        <v>192</v>
-      </c>
-      <c r="G1" t="n">
-        <v>3852849599.999999</v>
+          <t>tagid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intvalue</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>floatvalue</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>stringvalue</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>datevalue</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dataintegrity</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>t_stamp</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -573,7 +585,7 @@
         <v/>
       </c>
       <c r="C2" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v/>
@@ -585,7 +597,7 @@
         <v>192</v>
       </c>
       <c r="G2" t="n">
-        <v>3852852000</v>
+        <v>3852849599999.999</v>
       </c>
     </row>
     <row r="3">
@@ -598,7 +610,7 @@
         <v/>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="D3" t="n">
         <v/>
@@ -610,7 +622,7 @@
         <v>192</v>
       </c>
       <c r="G3" t="n">
-        <v>3852856800</v>
+        <v>3852853195000</v>
       </c>
     </row>
     <row r="4">
@@ -623,7 +635,7 @@
         <v/>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
         <v/>
@@ -635,7 +647,7 @@
         <v>192</v>
       </c>
       <c r="G4" t="n">
-        <v>3852860399.999999</v>
+        <v>3852856800000</v>
       </c>
     </row>
     <row r="5">
@@ -648,7 +660,7 @@
         <v/>
       </c>
       <c r="C5" t="n">
-        <v>18.5</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
         <v/>
@@ -660,7 +672,7 @@
         <v>192</v>
       </c>
       <c r="G5" t="n">
-        <v>3852861000</v>
+        <v>3852860399999.999</v>
       </c>
     </row>
     <row r="6">
@@ -685,7 +697,7 @@
         <v>192</v>
       </c>
       <c r="G6" t="n">
-        <v>3852864000.000001</v>
+        <v>3852864000000.001</v>
       </c>
     </row>
     <row r="7">
@@ -710,7 +722,7 @@
         <v>192</v>
       </c>
       <c r="G7" t="n">
-        <v>3852867600</v>
+        <v>3852867600000</v>
       </c>
     </row>
     <row r="8">
@@ -735,7 +747,7 @@
         <v>192</v>
       </c>
       <c r="G8" t="n">
-        <v>3852871199.999999</v>
+        <v>3852871199999.999</v>
       </c>
     </row>
     <row r="9">
@@ -760,7 +772,7 @@
         <v>192</v>
       </c>
       <c r="G9" t="n">
-        <v>3852874800.000001</v>
+        <v>3852874800000.001</v>
       </c>
     </row>
     <row r="10">
@@ -773,7 +785,7 @@
         <v/>
       </c>
       <c r="C10" t="n">
-        <v>50</v>
+        <v>53.5</v>
       </c>
       <c r="D10" t="n">
         <v/>
@@ -785,7 +797,7 @@
         <v>192</v>
       </c>
       <c r="G10" t="n">
-        <v>3852878400</v>
+        <v>3852878700000</v>
       </c>
     </row>
     <row r="11">
@@ -798,7 +810,7 @@
         <v/>
       </c>
       <c r="C11" t="n">
-        <v>57</v>
+        <v>58.75</v>
       </c>
       <c r="D11" t="n">
         <v/>
@@ -810,7 +822,7 @@
         <v>192</v>
       </c>
       <c r="G11" t="n">
-        <v>3852879000</v>
+        <v>3852881987000</v>
       </c>
     </row>
     <row r="12">
@@ -823,7 +835,7 @@
         <v/>
       </c>
       <c r="C12" t="n">
-        <v>60.5</v>
+        <v>64</v>
       </c>
       <c r="D12" t="n">
         <v/>
@@ -835,7 +847,7 @@
         <v>192</v>
       </c>
       <c r="G12" t="n">
-        <v>3852882000</v>
+        <v>3852885600000.001</v>
       </c>
     </row>
     <row r="13">
@@ -848,7 +860,7 @@
         <v/>
       </c>
       <c r="C13" t="n">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D13" t="n">
         <v/>
@@ -860,7 +872,7 @@
         <v>192</v>
       </c>
       <c r="G13" t="n">
-        <v>3852885600.000001</v>
+        <v>3852889200000</v>
       </c>
     </row>
     <row r="14">
@@ -873,7 +885,7 @@
         <v/>
       </c>
       <c r="C14" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D14" t="n">
         <v/>
@@ -885,7 +897,7 @@
         <v>192</v>
       </c>
       <c r="G14" t="n">
-        <v>3852889200</v>
+        <v>3852892799999.999</v>
       </c>
     </row>
     <row r="15">
@@ -898,7 +910,7 @@
         <v/>
       </c>
       <c r="C15" t="n">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D15" t="n">
         <v/>
@@ -910,7 +922,7 @@
         <v>192</v>
       </c>
       <c r="G15" t="n">
-        <v>3852892799.999999</v>
+        <v>3852896400000.001</v>
       </c>
     </row>
     <row r="16">
@@ -923,7 +935,7 @@
         <v/>
       </c>
       <c r="C16" t="n">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D16" t="n">
         <v/>
@@ -935,7 +947,7 @@
         <v>192</v>
       </c>
       <c r="G16" t="n">
-        <v>3852896400.000001</v>
+        <v>3852900000000</v>
       </c>
     </row>
     <row r="17">
@@ -948,7 +960,7 @@
         <v/>
       </c>
       <c r="C17" t="n">
-        <v>88.5</v>
+        <v>99</v>
       </c>
       <c r="D17" t="n">
         <v/>
@@ -960,7 +972,7 @@
         <v>192</v>
       </c>
       <c r="G17" t="n">
-        <v>3852897000</v>
+        <v>3852903599999.999</v>
       </c>
     </row>
     <row r="18">
@@ -973,7 +985,7 @@
         <v/>
       </c>
       <c r="C18" t="n">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D18" t="n">
         <v/>
@@ -985,7 +997,7 @@
         <v>192</v>
       </c>
       <c r="G18" t="n">
-        <v>3852900000</v>
+        <v>3852907200000.001</v>
       </c>
     </row>
     <row r="19">
@@ -998,7 +1010,7 @@
         <v/>
       </c>
       <c r="C19" t="n">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D19" t="n">
         <v/>
@@ -1010,7 +1022,7 @@
         <v>192</v>
       </c>
       <c r="G19" t="n">
-        <v>3852903599.999999</v>
+        <v>3852910800000</v>
       </c>
     </row>
     <row r="20">
@@ -1023,7 +1035,7 @@
         <v/>
       </c>
       <c r="C20" t="n">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="D20" t="n">
         <v/>
@@ -1035,7 +1047,7 @@
         <v>192</v>
       </c>
       <c r="G20" t="n">
-        <v>3852907200.000001</v>
+        <v>3852914399999.999</v>
       </c>
     </row>
     <row r="21">
@@ -1048,7 +1060,7 @@
         <v/>
       </c>
       <c r="C21" t="n">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D21" t="n">
         <v/>
@@ -1060,7 +1072,7 @@
         <v>192</v>
       </c>
       <c r="G21" t="n">
-        <v>3852910800</v>
+        <v>3852918000000.001</v>
       </c>
     </row>
     <row r="22">
@@ -1073,7 +1085,7 @@
         <v/>
       </c>
       <c r="C22" t="n">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D22" t="n">
         <v/>
@@ -1085,7 +1097,7 @@
         <v>192</v>
       </c>
       <c r="G22" t="n">
-        <v>3852914399.999999</v>
+        <v>3852921600000</v>
       </c>
     </row>
     <row r="23">
@@ -1098,7 +1110,7 @@
         <v/>
       </c>
       <c r="C23" t="n">
-        <v>123.5</v>
+        <v>141</v>
       </c>
       <c r="D23" t="n">
         <v/>
@@ -1110,7 +1122,7 @@
         <v>192</v>
       </c>
       <c r="G23" t="n">
-        <v>3852915000</v>
+        <v>3852925199999.999</v>
       </c>
     </row>
     <row r="24">
@@ -1123,7 +1135,7 @@
         <v/>
       </c>
       <c r="C24" t="n">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="D24" t="n">
         <v/>
@@ -1135,7 +1147,7 @@
         <v>192</v>
       </c>
       <c r="G24" t="n">
-        <v>3852918000.000001</v>
+        <v>3852928800000.001</v>
       </c>
     </row>
     <row r="25">
@@ -1148,7 +1160,7 @@
         <v/>
       </c>
       <c r="C25" t="n">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D25" t="n">
         <v/>
@@ -1160,7 +1172,7 @@
         <v>192</v>
       </c>
       <c r="G25" t="n">
-        <v>3852921600</v>
+        <v>3852932400000</v>
       </c>
     </row>
     <row r="26">
@@ -1173,7 +1185,7 @@
         <v/>
       </c>
       <c r="C26" t="n">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="D26" t="n">
         <v/>
@@ -1185,7 +1197,7 @@
         <v>192</v>
       </c>
       <c r="G26" t="n">
-        <v>3852925199.999999</v>
+        <v>3852935999999.999</v>
       </c>
     </row>
     <row r="27">
@@ -1198,7 +1210,7 @@
         <v/>
       </c>
       <c r="C27" t="n">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="D27" t="n">
         <v/>
@@ -1210,107 +1222,7 @@
         <v>192</v>
       </c>
       <c r="G27" t="n">
-        <v>3852928800.000001</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v/>
-      </c>
-      <c r="C28" t="n">
-        <v>155</v>
-      </c>
-      <c r="D28" t="n">
-        <v/>
-      </c>
-      <c r="E28" t="n">
-        <v/>
-      </c>
-      <c r="F28" t="n">
-        <v>192</v>
-      </c>
-      <c r="G28" t="n">
-        <v>3852932400</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v/>
-      </c>
-      <c r="C29" t="n">
-        <v>162</v>
-      </c>
-      <c r="D29" t="n">
-        <v/>
-      </c>
-      <c r="E29" t="n">
-        <v/>
-      </c>
-      <c r="F29" t="n">
-        <v>192</v>
-      </c>
-      <c r="G29" t="n">
-        <v>3852935999.999999</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v/>
-      </c>
-      <c r="C30" t="n">
-        <v>165.5</v>
-      </c>
-      <c r="D30" t="n">
-        <v/>
-      </c>
-      <c r="E30" t="n">
-        <v/>
-      </c>
-      <c r="F30" t="n">
-        <v>192</v>
-      </c>
-      <c r="G30" t="n">
-        <v>3852936000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v/>
-      </c>
-      <c r="C31" t="n">
-        <v>169</v>
-      </c>
-      <c r="D31" t="n">
-        <v/>
-      </c>
-      <c r="E31" t="n">
-        <v/>
-      </c>
-      <c r="F31" t="n">
-        <v>192</v>
-      </c>
-      <c r="G31" t="n">
-        <v>3852939600.000001</v>
+        <v>3852939600000.001</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,17 +1247,38 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" t="n">
-        <v>192</v>
-      </c>
-      <c r="G1" t="n">
-        <v>3852849599.999999</v>
+          <t>tagid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intvalue</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>floatvalue</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>stringvalue</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>datevalue</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dataintegrity</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>t_stamp</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1355,13 +1288,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>192</v>
       </c>
       <c r="G2" t="n">
-        <v>3852856800</v>
+        <v>3852849599999.999</v>
       </c>
     </row>
     <row r="3">
@@ -1371,13 +1304,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>192</v>
       </c>
       <c r="G3" t="n">
-        <v>3852860399.999999</v>
+        <v>3852856800000</v>
       </c>
     </row>
     <row r="4">
@@ -1393,7 +1326,7 @@
         <v>192</v>
       </c>
       <c r="G4" t="n">
-        <v>3852864000.000001</v>
+        <v>3852860399999.999</v>
       </c>
     </row>
     <row r="5">
@@ -1409,7 +1342,7 @@
         <v>192</v>
       </c>
       <c r="G5" t="n">
-        <v>3852867600</v>
+        <v>3852864000000.001</v>
       </c>
     </row>
     <row r="6">
@@ -1425,7 +1358,7 @@
         <v>192</v>
       </c>
       <c r="G6" t="n">
-        <v>3852871199.999999</v>
+        <v>3852867600000</v>
       </c>
     </row>
     <row r="7">
@@ -1441,7 +1374,7 @@
         <v>192</v>
       </c>
       <c r="G7" t="n">
-        <v>3852874800.000001</v>
+        <v>3852871199999.999</v>
       </c>
     </row>
     <row r="8">
@@ -1457,7 +1390,7 @@
         <v>192</v>
       </c>
       <c r="G8" t="n">
-        <v>3852878400</v>
+        <v>3852874800000.001</v>
       </c>
     </row>
     <row r="9">
@@ -1473,7 +1406,7 @@
         <v>192</v>
       </c>
       <c r="G9" t="n">
-        <v>3852879000</v>
+        <v>3852878400000</v>
       </c>
     </row>
     <row r="10">
@@ -1489,7 +1422,7 @@
         <v>192</v>
       </c>
       <c r="G10" t="n">
-        <v>3852885600.000001</v>
+        <v>3852879000000</v>
       </c>
     </row>
     <row r="11">
@@ -1505,7 +1438,7 @@
         <v>192</v>
       </c>
       <c r="G11" t="n">
-        <v>3852889200</v>
+        <v>3852885600000.001</v>
       </c>
     </row>
     <row r="12">
@@ -1521,7 +1454,7 @@
         <v>192</v>
       </c>
       <c r="G12" t="n">
-        <v>3852892799.999999</v>
+        <v>3852889200000</v>
       </c>
     </row>
     <row r="13">
@@ -1537,7 +1470,7 @@
         <v>192</v>
       </c>
       <c r="G13" t="n">
-        <v>3852896400.000001</v>
+        <v>3852892799999.999</v>
       </c>
     </row>
     <row r="14">
@@ -1553,7 +1486,7 @@
         <v>192</v>
       </c>
       <c r="G14" t="n">
-        <v>3852900000</v>
+        <v>3852896400000.001</v>
       </c>
     </row>
     <row r="15">
@@ -1569,7 +1502,7 @@
         <v>192</v>
       </c>
       <c r="G15" t="n">
-        <v>3852903599.999999</v>
+        <v>3852900000000</v>
       </c>
     </row>
     <row r="16">
@@ -1585,7 +1518,7 @@
         <v>192</v>
       </c>
       <c r="G16" t="n">
-        <v>3852907200.000001</v>
+        <v>3852903599999.999</v>
       </c>
     </row>
     <row r="17">
@@ -1601,7 +1534,7 @@
         <v>192</v>
       </c>
       <c r="G17" t="n">
-        <v>3852910800</v>
+        <v>3852907200000.001</v>
       </c>
     </row>
     <row r="18">
@@ -1617,7 +1550,7 @@
         <v>192</v>
       </c>
       <c r="G18" t="n">
-        <v>3852914399.999999</v>
+        <v>3852910800000</v>
       </c>
     </row>
     <row r="19">
@@ -1633,7 +1566,7 @@
         <v>192</v>
       </c>
       <c r="G19" t="n">
-        <v>3852918000.000001</v>
+        <v>3852914399999.999</v>
       </c>
     </row>
     <row r="20">
@@ -1649,7 +1582,7 @@
         <v>192</v>
       </c>
       <c r="G20" t="n">
-        <v>3852921600</v>
+        <v>3852918000000.001</v>
       </c>
     </row>
     <row r="21">
@@ -1665,7 +1598,7 @@
         <v>192</v>
       </c>
       <c r="G21" t="n">
-        <v>3852925199.999999</v>
+        <v>3852921600000</v>
       </c>
     </row>
     <row r="22">
@@ -1681,7 +1614,7 @@
         <v>192</v>
       </c>
       <c r="G22" t="n">
-        <v>3852928800.000001</v>
+        <v>3852925199999.999</v>
       </c>
     </row>
     <row r="23">
@@ -1697,7 +1630,7 @@
         <v>192</v>
       </c>
       <c r="G23" t="n">
-        <v>3852932400</v>
+        <v>3852928800000.001</v>
       </c>
     </row>
     <row r="24">
@@ -1713,7 +1646,7 @@
         <v>192</v>
       </c>
       <c r="G24" t="n">
-        <v>3852935999.999999</v>
+        <v>3852932400000</v>
       </c>
     </row>
     <row r="25">
@@ -1729,7 +1662,23 @@
         <v>192</v>
       </c>
       <c r="G25" t="n">
-        <v>3852939600.000001</v>
+        <v>3852935999999.999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>192</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3852939600000.001</v>
       </c>
     </row>
   </sheetData>
@@ -1746,12 +1695,12 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35"/>
   <cols>
-    <col width="13.05859375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="16.8203125" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="13.05859375" bestFit="1" customWidth="1" min="10" max="10"/>
     <col width="15" bestFit="1" customWidth="1" min="13" max="13"/>
     <col width="14.3515625" bestFit="1" customWidth="1" min="16" max="16"/>
@@ -1875,7 +1824,7 @@
         <v>192</v>
       </c>
       <c r="G2" s="13">
-        <f>P2</f>
+        <f>P2*1000</f>
         <v/>
       </c>
       <c r="H2" s="14" t="n"/>
@@ -1946,7 +1895,7 @@
         <v>192</v>
       </c>
       <c r="G3" s="13">
-        <f>P3</f>
+        <f>P3*1000</f>
         <v/>
       </c>
       <c r="H3" s="14" t="n"/>
@@ -2031,7 +1980,7 @@
         <v>192</v>
       </c>
       <c r="G4" s="13">
-        <f>P4</f>
+        <f>P4*1000</f>
         <v/>
       </c>
       <c r="H4" s="14" t="n"/>
@@ -2116,7 +2065,7 @@
         <v>192</v>
       </c>
       <c r="G5" s="13">
-        <f>P5</f>
+        <f>P5*1000</f>
         <v/>
       </c>
       <c r="H5" s="14" t="n"/>
@@ -2194,7 +2143,7 @@
         <v>192</v>
       </c>
       <c r="G6" s="13">
-        <f>P6</f>
+        <f>P6*1000</f>
         <v/>
       </c>
       <c r="H6" s="14" t="n"/>
@@ -2272,7 +2221,7 @@
         <v>192</v>
       </c>
       <c r="G7" s="13">
-        <f>P7</f>
+        <f>P7*1000</f>
         <v/>
       </c>
       <c r="H7" s="14" t="n"/>
@@ -2350,7 +2299,7 @@
         <v>192</v>
       </c>
       <c r="G8" s="13">
-        <f>P8</f>
+        <f>P8*1000</f>
         <v/>
       </c>
       <c r="H8" s="14" t="n"/>
@@ -2428,7 +2377,7 @@
         <v>192</v>
       </c>
       <c r="G9" s="13">
-        <f>P9</f>
+        <f>P9*1000</f>
         <v/>
       </c>
       <c r="H9" s="14" t="n"/>
@@ -2506,7 +2455,7 @@
         <v>192</v>
       </c>
       <c r="G10" s="13">
-        <f>P10</f>
+        <f>P10*1000</f>
         <v/>
       </c>
       <c r="H10" s="14" t="n"/>
@@ -2584,7 +2533,7 @@
         <v>192</v>
       </c>
       <c r="G11" s="13">
-        <f>P11</f>
+        <f>P11*1000</f>
         <v/>
       </c>
       <c r="H11" s="14" t="n"/>
@@ -2662,7 +2611,7 @@
         <v>192</v>
       </c>
       <c r="G12" s="13">
-        <f>P12</f>
+        <f>P12*1000</f>
         <v/>
       </c>
       <c r="H12" s="14" t="n"/>
@@ -2740,7 +2689,7 @@
         <v>192</v>
       </c>
       <c r="G13" s="13">
-        <f>P13</f>
+        <f>P13*1000</f>
         <v/>
       </c>
       <c r="H13" s="14" t="n"/>
@@ -2818,7 +2767,7 @@
         <v>192</v>
       </c>
       <c r="G14" s="13">
-        <f>P14</f>
+        <f>P14*1000</f>
         <v/>
       </c>
       <c r="H14" s="14" t="n"/>
@@ -2896,7 +2845,7 @@
         <v>192</v>
       </c>
       <c r="G15" s="13">
-        <f>P15</f>
+        <f>P15*1000</f>
         <v/>
       </c>
       <c r="H15" s="14" t="n"/>
@@ -2974,7 +2923,7 @@
         <v>192</v>
       </c>
       <c r="G16" s="13">
-        <f>P16</f>
+        <f>P16*1000</f>
         <v/>
       </c>
       <c r="H16" s="14" t="n"/>
@@ -3052,7 +3001,7 @@
         <v>192</v>
       </c>
       <c r="G17" s="13">
-        <f>P17</f>
+        <f>P17*1000</f>
         <v/>
       </c>
       <c r="H17" s="14" t="n"/>
@@ -3130,7 +3079,7 @@
         <v>192</v>
       </c>
       <c r="G18" s="13">
-        <f>P18</f>
+        <f>P18*1000</f>
         <v/>
       </c>
       <c r="H18" s="14" t="n"/>
@@ -3208,7 +3157,7 @@
         <v>192</v>
       </c>
       <c r="G19" s="13">
-        <f>P19</f>
+        <f>P19*1000</f>
         <v/>
       </c>
       <c r="H19" s="14" t="n"/>
@@ -3286,7 +3235,7 @@
         <v>192</v>
       </c>
       <c r="G20" s="13">
-        <f>P20</f>
+        <f>P20*1000</f>
         <v/>
       </c>
       <c r="H20" s="14" t="n"/>
@@ -3364,7 +3313,7 @@
         <v>192</v>
       </c>
       <c r="G21" s="13">
-        <f>P21</f>
+        <f>P21*1000</f>
         <v/>
       </c>
       <c r="H21" s="14" t="n"/>
@@ -3442,7 +3391,7 @@
         <v>192</v>
       </c>
       <c r="G22" s="13">
-        <f>P22</f>
+        <f>P22*1000</f>
         <v/>
       </c>
       <c r="H22" s="14" t="n"/>
@@ -3520,7 +3469,7 @@
         <v>192</v>
       </c>
       <c r="G23" s="13">
-        <f>P23</f>
+        <f>P23*1000</f>
         <v/>
       </c>
       <c r="H23" s="14" t="n"/>
@@ -3598,7 +3547,7 @@
         <v>192</v>
       </c>
       <c r="G24" s="13">
-        <f>P24</f>
+        <f>P24*1000</f>
         <v/>
       </c>
       <c r="H24" s="14" t="n"/>
@@ -3676,7 +3625,7 @@
         <v>192</v>
       </c>
       <c r="G25" s="13">
-        <f>P25</f>
+        <f>P25*1000</f>
         <v/>
       </c>
       <c r="H25" s="14" t="n"/>
@@ -3754,7 +3703,7 @@
         <v>192</v>
       </c>
       <c r="G26" s="13">
-        <f>P26</f>
+        <f>P26*1000</f>
         <v/>
       </c>
       <c r="H26" s="14" t="n"/>

</xml_diff>